<commit_message>
Add 21th_day_test and 60th_day_test into Estrus.
</commit_message>
<xml_diff>
--- a/test/reader/dong_ying/parents_output.xlsx
+++ b/test/reader/dong_ying/parents_output.xlsx
@@ -441,7 +441,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,74 +452,86 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="n">
-        <v>190602</v>
-      </c>
-      <c r="C1" t="n">
-        <v>110602</v>
-      </c>
-      <c r="D1" s="2" t="n">
-        <v>43068</v>
+          <t>Breed</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>confusing_note</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Birthday</t>
+        </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Y168607王</t>
+          <t>Sire</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Y128405韓</t>
-        </is>
-      </c>
-      <c r="G1" t="n">
-        <v>231754</v>
+          <t>Dam</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>reg_id</t>
+        </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>王韓</t>
+          <t>Chinese_name</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>母</t>
+          <t>Gender</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>['不允許有相近耳號']</t>
+          <t>註釋</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>194303</v>
+        <v>190602</v>
       </c>
       <c r="C2" t="n">
-        <v>114303</v>
+        <v>110602</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>43105</v>
-      </c>
-      <c r="E2" t="n">
-        <v/>
-      </c>
-      <c r="F2" t="n">
-        <v/>
+        <v>43068</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Y168607王</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Y128405韓</t>
+        </is>
       </c>
       <c r="G2" t="n">
-        <v>231762</v>
+        <v>231754</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>趙花</t>
+          <t>王韓</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -540,30 +552,26 @@
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>197402</v>
+        <v>194303</v>
       </c>
       <c r="C3" t="n">
-        <v>197401</v>
+        <v>114303</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>43160</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>L156009桃</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>L155804秦</t>
-        </is>
+        <v>43105</v>
+      </c>
+      <c r="E3" t="n">
+        <v/>
+      </c>
+      <c r="F3" t="n">
+        <v/>
       </c>
       <c r="G3" t="n">
-        <v>231844</v>
+        <v>231762</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>桃秦</t>
+          <t>趙花</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -584,30 +592,30 @@
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>115501</v>
+        <v>197402</v>
       </c>
       <c r="C4" t="n">
-        <v>195509</v>
+        <v>197401</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>43468</v>
+        <v>43160</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>L107111仁</t>
+          <t>L156009桃</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>L171903愛</t>
+          <t>L155804秦</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>234141</v>
+        <v>231844</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>仁愛</t>
+          <t>桃秦</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -628,30 +636,30 @@
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>116403</v>
+        <v>115501</v>
       </c>
       <c r="C5" t="n">
-        <v>196403</v>
+        <v>195509</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>43478</v>
+        <v>43468</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>L117009桃</t>
+          <t>L107111仁</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>L181704齊</t>
+          <t>L171903愛</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>234972</v>
+        <v>234141</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>桃傑</t>
+          <t>仁愛</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -668,34 +676,34 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>L</t>
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>117306</v>
+        <v>116403</v>
       </c>
       <c r="C6" t="n">
-        <v>117906</v>
+        <v>196403</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>43495</v>
+        <v>43478</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Y135604趙</t>
+          <t>L117009桃</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Y130104合</t>
+          <t>L181704齊</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>234125</v>
+        <v>234972</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>趙合</t>
+          <t>桃傑</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -712,34 +720,34 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="B7" s="1" t="n">
-        <v>122001</v>
+        <v>117306</v>
       </c>
       <c r="C7" t="n">
-        <v>122009</v>
+        <v>117906</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>43565</v>
+        <v>43495</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>L195003桃</t>
+          <t>Y135604趙</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>L152103楚</t>
+          <t>Y130104合</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>234156</v>
+        <v>234125</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>桃楚</t>
+          <t>趙合</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -756,34 +764,34 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>L</t>
         </is>
       </c>
       <c r="B8" s="1" t="n">
-        <v>124403</v>
+        <v>122001</v>
       </c>
       <c r="C8" t="n">
-        <v>124303</v>
+        <v>122009</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>43608</v>
+        <v>43565</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Y153804德</t>
+          <t>L195003桃</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Y134101聖</t>
+          <t>L152103楚</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>236729</v>
+        <v>234156</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>德聖</t>
+          <t>桃楚</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -800,34 +808,34 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="B9" s="1" t="n">
-        <v>126714</v>
+        <v>124403</v>
       </c>
       <c r="C9" t="n">
-        <v>122714</v>
+        <v>124303</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>43649</v>
+        <v>43608</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>L180809齊</t>
+          <t>Y153804德</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>L163601傑</t>
+          <t>Y134101聖</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>237148</v>
+        <v>236729</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>齊傑</t>
+          <t>德聖</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -844,37 +852,35 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>L</t>
         </is>
       </c>
       <c r="B10" s="1" t="n">
-        <v>127505</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>L?</t>
-        </is>
+        <v>126714</v>
+      </c>
+      <c r="C10" t="n">
+        <v>122714</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>43658</v>
+        <v>43649</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>L167111仁</t>
+          <t>L180809齊</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>L180603愛</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>無登</t>
-        </is>
-      </c>
-      <c r="H10" t="n">
-        <v/>
+          <t>L163601傑</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>237148</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>齊傑</t>
+        </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -883,7 +889,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>['{field} 不能為空值', '不允許有相近耳號']</t>
+          <t>['不允許有相近耳號']</t>
         </is>
       </c>
     </row>
@@ -893,27 +899,25 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="B11" s="1" t="inlineStr">
-        <is>
-          <t>142701</t>
-        </is>
+      <c r="B11" s="1" t="n">
+        <v>127505</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>相近耳號</t>
+          <t>L?</t>
         </is>
       </c>
       <c r="D11" s="2" t="n">
-        <v>43910</v>
+        <v>43658</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Y185809趙</t>
+          <t>L167111仁</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Y182801德</t>
+          <t>L180603愛</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -921,19 +925,17 @@
           <t>無登</t>
         </is>
       </c>
-      <c r="H11" s="1" t="inlineStr">
-        <is>
-          <t>趙德</t>
-        </is>
+      <c r="H11" t="n">
+        <v/>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>母/公</t>
+          <t>母</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>['"性別 母/公 錯誤。性別需定義於下表：\\n{\'公\': \'M\', \'母\': \'F\', \'M\': \'M\', \'F\': \'F\', \'1\': \'M\', \'2\': \'F\'}"', '不允許有相近耳號']</t>
+          <t>['Chinese_name 不能為空值', '不允許有相近耳號']</t>
         </is>
       </c>
     </row>
@@ -943,41 +945,47 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="B12" s="1" t="n">
-        <v>142509</v>
-      </c>
-      <c r="C12" t="n">
-        <v>142905</v>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>142701</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>相近耳號</t>
+        </is>
       </c>
       <c r="D12" s="2" t="n">
-        <v>43915</v>
+        <v>43910</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Y104206趙</t>
+          <t>Y185809趙</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Y160505花</t>
-        </is>
-      </c>
-      <c r="G12" t="n">
-        <v>238793</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>趙金</t>
+          <t>Y182801德</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>無登</t>
+        </is>
+      </c>
+      <c r="H12" s="1" t="inlineStr">
+        <is>
+          <t>趙德</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>母</t>
+          <t>母/公</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>['不允許有相近耳號']</t>
+          <t>['"性別 母/公 錯誤。性別需定義於下表：\\n{\'公\': \'M\', \'母\': \'F\', \'M\': \'M\', \'F\': \'F\', \'1\': \'M\', \'2\': \'F\'}"', '不允許有相近耳號']</t>
         </is>
       </c>
     </row>
@@ -988,17 +996,17 @@
         </is>
       </c>
       <c r="B13" s="1" t="n">
-        <v>151103</v>
+        <v>142509</v>
       </c>
       <c r="C13" t="n">
-        <v>159403</v>
+        <v>142905</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>44056</v>
+        <v>43915</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Y121005地</t>
+          <t>Y104206趙</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1007,11 +1015,11 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>241446</v>
+        <v>238793</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>地花</t>
+          <t>趙金</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1028,34 +1036,34 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="B14" s="1" t="n">
-        <v>155202</v>
+        <v>151103</v>
       </c>
       <c r="C14" t="n">
-        <v>155102</v>
+        <v>159403</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>44111</v>
+        <v>44056</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>L180607愛</t>
+          <t>Y121005地</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>L187903燕</t>
+          <t>Y160505花</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>243024</v>
+        <v>241446</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>愛燕</t>
+          <t>地花</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1076,32 +1084,30 @@
         </is>
       </c>
       <c r="B15" s="1" t="n">
-        <v>159607</v>
+        <v>155202</v>
       </c>
       <c r="C15" t="n">
-        <v>149607</v>
+        <v>155102</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>44188</v>
+        <v>44111</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>L156208傑</t>
+          <t>L180607愛</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>L195405仁</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>無登</t>
-        </is>
+          <t>L187903燕</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>243024</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>傑仁</t>
+          <t>愛燕</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1118,34 +1124,36 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>L</t>
         </is>
       </c>
       <c r="B16" s="1" t="n">
-        <v>161202</v>
+        <v>159607</v>
       </c>
       <c r="C16" t="n">
-        <v>161203</v>
+        <v>149607</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>44210</v>
+        <v>44188</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Y121005地</t>
+          <t>L156208傑</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Y107903花</t>
-        </is>
-      </c>
-      <c r="G16" t="n">
-        <v>241463</v>
+          <t>L195405仁</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>無登</t>
+        </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>地花</t>
+          <t>傑仁</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1162,41 +1170,39 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="B17" s="1" t="n">
-        <v>163603</v>
+        <v>161202</v>
       </c>
       <c r="C17" t="n">
-        <v>163609</v>
+        <v>161203</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>44258</v>
+        <v>44210</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>L156208傑</t>
+          <t>Y121005地</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>L191603仁</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>無登</t>
-        </is>
+          <t>Y107903花</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>241463</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>傑仁</t>
+          <t>地花</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>公</t>
+          <t>母</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1208,26 +1214,26 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>L</t>
         </is>
       </c>
       <c r="B18" s="1" t="n">
-        <v>167602</v>
+        <v>163603</v>
       </c>
       <c r="C18" t="n">
-        <v>156602</v>
+        <v>163609</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>44336</v>
+        <v>44258</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Y114110趙</t>
+          <t>L156208傑</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Y109303地</t>
+          <t>L191603仁</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1237,12 +1243,12 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>趙地</t>
+          <t>傑仁</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>母</t>
+          <t>公</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1258,30 +1264,32 @@
         </is>
       </c>
       <c r="B19" s="1" t="n">
-        <v>170005</v>
+        <v>167602</v>
       </c>
       <c r="C19" t="n">
-        <v>170003</v>
+        <v>156602</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>44370</v>
+        <v>44336</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Y147505金</t>
+          <t>Y114110趙</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Y199603地</t>
-        </is>
-      </c>
-      <c r="G19" t="n">
-        <v>243044</v>
+          <t>Y109303地</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>無登</t>
+        </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>金地</t>
+          <t>趙地</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1302,32 +1310,30 @@
         </is>
       </c>
       <c r="B20" s="1" t="n">
-        <v>173505</v>
+        <v>170005</v>
       </c>
       <c r="C20" t="n">
-        <v>173503</v>
+        <v>170003</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>44426</v>
+        <v>44370</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Y141309王</t>
+          <t>Y147505金</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Y124706地</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>無登</t>
-        </is>
+          <t>Y199603地</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>243044</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>王地</t>
+          <t>金地</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1344,34 +1350,36 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="B21" s="1" t="n">
-        <v>175103</v>
+        <v>173505</v>
       </c>
       <c r="C21" t="n">
-        <v>175104</v>
+        <v>173503</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>44447</v>
+        <v>44426</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>L149407傑</t>
+          <t>Y141309王</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>L117902愛</t>
-        </is>
-      </c>
-      <c r="G21" t="n">
-        <v>243038</v>
+          <t>Y124706地</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>無登</t>
+        </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>傑愛</t>
+          <t>王地</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1388,36 +1396,34 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>L</t>
         </is>
       </c>
       <c r="B22" s="1" t="n">
-        <v>177107</v>
+        <v>175103</v>
       </c>
       <c r="C22" t="n">
-        <v>175107</v>
+        <v>175104</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>44475</v>
+        <v>44447</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Y121005地</t>
+          <t>L149407傑</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Y102703王</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>無登</t>
-        </is>
+          <t>L117902愛</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>243038</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>無登</t>
+          <t>傑愛</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1434,26 +1440,26 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="B23" s="1" t="n">
-        <v>178703</v>
+        <v>177107</v>
       </c>
       <c r="C23" t="n">
-        <v>178709</v>
+        <v>175107</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>44496</v>
+        <v>44475</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>L146907齊</t>
+          <t>Y121005地</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>L126601楚</t>
+          <t>Y102703王</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1463,7 +1469,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>齊楚</t>
+          <t>無登</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1494,7 +1500,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>L146407齊</t>
+          <t>L146907齊</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1526,26 +1532,26 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>L</t>
         </is>
       </c>
       <c r="B25" s="1" t="n">
-        <v>179103</v>
+        <v>178703</v>
       </c>
       <c r="C25" t="n">
-        <v>179003</v>
+        <v>178709</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>44503</v>
+        <v>44496</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Y149212德</t>
+          <t>L146407齊</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Y110904王</t>
+          <t>L126601楚</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1555,7 +1561,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>德王</t>
+          <t>齊楚</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1576,42 +1582,88 @@
         </is>
       </c>
       <c r="B26" s="1" t="n">
+        <v>179103</v>
+      </c>
+      <c r="C26" t="n">
+        <v>179003</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>44503</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Y149212德</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Y110904王</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>無登</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>德王</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>母</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>['不允許有相近耳號']</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="n">
         <v>179305</v>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>L?</t>
         </is>
       </c>
-      <c r="D26" s="2" t="n">
+      <c r="D27" s="2" t="n">
         <v>44504</v>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>L149412傑</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>L104301楚</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="G27" t="inlineStr">
         <is>
           <t>無登</t>
         </is>
       </c>
-      <c r="H26" t="n">
+      <c r="H27" t="n">
         <v/>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>母</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>['{field} 不能為空值', '不允許有相近耳號']</t>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>母</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>['Chinese_name 不能為空值', '不允許有相近耳號']</t>
         </is>
       </c>
     </row>

</xml_diff>